<commit_message>
Test out SPS chapter advisor update logic
The Harvard-Marlboro problem even persists with the chapter advisor update. It's A PROBLEM.
</commit_message>
<xml_diff>
--- a/Updated Zone 1 Activity New.xlsx
+++ b/Updated Zone 1 Activity New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B94296C-C460-4B4F-88B0-ED288EE7CA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46B8C39-760D-0440-B444-CCA8CE896959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="818">
   <si>
     <t>Member/Non-Member - Organization</t>
   </si>
@@ -1372,354 +1372,276 @@
     <t>s.kar@neu.edu</t>
   </si>
   <si>
-    <t>Professor Rudra Kafle</t>
-  </si>
-  <si>
-    <t>Kristina A. Lynch</t>
-  </si>
-  <si>
-    <t>Robert Cordery</t>
-  </si>
-  <si>
-    <t>David Morin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joe Checkelsky
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spencer Smith
-</t>
-  </si>
-  <si>
-    <t>Professor William Karstens</t>
-  </si>
-  <si>
-    <t>Joyce Palmer-Fortune</t>
+    <t xml:space="preserve">Angela Biselli and Robert Cordery </t>
+  </si>
+  <si>
+    <t>Prof. Joe Checkelsky</t>
+  </si>
+  <si>
+    <t>Spencer Smith</t>
+  </si>
+  <si>
+    <t>Joyce Palmer Fortune</t>
+  </si>
+  <si>
+    <t>Timothy Atherton</t>
+  </si>
+  <si>
+    <t>Frank Dudish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professor Rudra </t>
+  </si>
+  <si>
+    <t>Sarah Demers</t>
+  </si>
+  <si>
+    <t>Matthew Guthrie</t>
+  </si>
+  <si>
+    <t>Ben Heidenreich</t>
+  </si>
+  <si>
+    <t>Dr. David Morin</t>
+  </si>
+  <si>
+    <t>David Kagan</t>
+  </si>
+  <si>
+    <t>checkelsky@mit.edu</t>
+  </si>
+  <si>
+    <t>smiths@mtholyoke.edu</t>
+  </si>
+  <si>
+    <t>timothy.atherton@tufts.edu</t>
+  </si>
+  <si>
+    <t>frank.dudish@maine.edu</t>
+  </si>
+  <si>
+    <t>rpk101@wpi.edu</t>
+  </si>
+  <si>
+    <t>sarah.demerskonezny@yale.edu</t>
+  </si>
+  <si>
+    <t>bheidenreich@umass.edu</t>
+  </si>
+  <si>
+    <t>dkagan@umassd.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Charles Thomas Hess</t>
+  </si>
+  <si>
+    <t>Greg Voth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hess@maine.edu</t>
+  </si>
+  <si>
+    <t>gvoth@wesleyan.edu</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Disbanded</t>
+  </si>
+  <si>
+    <t>Michael Graf</t>
+  </si>
+  <si>
+    <t>Vesna Mitrović​​</t>
+  </si>
+  <si>
+    <t>James LaBelle</t>
+  </si>
+  <si>
+    <t>Professor Brother Jonathan Stott, S.J.</t>
+  </si>
+  <si>
+    <t>Cumrun Vafa</t>
+  </si>
+  <si>
+    <t>Raymond Ashoori</t>
+  </si>
+  <si>
+    <t>Ian Durham</t>
+  </si>
+  <si>
+    <t>Alain Brizard</t>
+  </si>
+  <si>
+    <t>Nathanael Fortune</t>
   </si>
   <si>
     <t>Dr. Walter Johnson</t>
   </si>
   <si>
-    <t>Frank Dudish</t>
-  </si>
-  <si>
-    <t>Sumientra Rampersad</t>
-  </si>
-  <si>
-    <t>Dr. Benjamin Chandran</t>
-  </si>
-  <si>
-    <t>Rudra Kafle</t>
-  </si>
-  <si>
-    <t>Sarah Demers</t>
-  </si>
-  <si>
-    <t>William Loinaz</t>
-  </si>
-  <si>
-    <t>Robert Carey</t>
-  </si>
-  <si>
-    <t>Dr. Thayaparan Paramanathan</t>
-  </si>
-  <si>
-    <t>Thomas Burton</t>
-  </si>
-  <si>
-    <t>Joseph Ribaudo</t>
-  </si>
-  <si>
-    <t>Matt Guthrie</t>
-  </si>
-  <si>
-    <t>Ben Brau</t>
-  </si>
-  <si>
-    <t>John Smedley</t>
-  </si>
-  <si>
-    <t>Mark O. Battle</t>
-  </si>
-  <si>
-    <t>Richard Fell</t>
-  </si>
-  <si>
-    <t>Dr. Michael Boyer</t>
-  </si>
-  <si>
-    <t>Dr. Michael Weinstein</t>
-  </si>
-  <si>
-    <t>Dr. Cornely</t>
+    <t>Barbara Walden</t>
+  </si>
+  <si>
+    <t>Lawrence Ford</t>
+  </si>
+  <si>
+    <t>John Thompson</t>
+  </si>
+  <si>
+    <t>Rahul Kulkarni</t>
+  </si>
+  <si>
+    <t>Arthur Mittler</t>
+  </si>
+  <si>
+    <t>Per Berglund</t>
+  </si>
+  <si>
+    <t>Randall Headrick</t>
+  </si>
+  <si>
+    <t>Doug Petkie</t>
+  </si>
+  <si>
+    <t>Karsten Heeger</t>
+  </si>
+  <si>
+    <t>David Hanneke</t>
+  </si>
+  <si>
+    <t>Andrei Ruckenstein</t>
+  </si>
+  <si>
+    <t>Tom Kling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kebra Ward </t>
+  </si>
+  <si>
+    <t>Seth Ashman</t>
+  </si>
+  <si>
+    <t>George Gibson</t>
+  </si>
+  <si>
+    <t>Anthony Dinsmore</t>
+  </si>
+  <si>
+    <t>John Michael Collins</t>
+  </si>
+  <si>
+    <t>Travis Gould</t>
+  </si>
+  <si>
+    <t>Steve Naculich</t>
+  </si>
+  <si>
+    <t>Jane' Kondev</t>
+  </si>
+  <si>
+    <t>Peter LeMaire</t>
+  </si>
+  <si>
+    <t>Arshad Kudrolli</t>
+  </si>
+  <si>
+    <t>Tom Narita</t>
+  </si>
+  <si>
+    <t>Pierre-Richard Cornely</t>
   </si>
   <si>
     <t>David Lee</t>
   </si>
   <si>
-    <t>Dr. Steven Harfenist</t>
-  </si>
-  <si>
-    <t>Richard Hyde</t>
-  </si>
-  <si>
-    <t>Nancy Lee</t>
-  </si>
-  <si>
-    <t>Sps Advisor</t>
-  </si>
-  <si>
-    <t>Loraine Allen</t>
-  </si>
-  <si>
-    <t>James McDonald</t>
+    <t>Steven Harfenist</t>
+  </si>
+  <si>
+    <t>Sara Salimbeni</t>
+  </si>
+  <si>
+    <t>Craig Looney</t>
+  </si>
+  <si>
+    <t>Anne Goodsell</t>
+  </si>
+  <si>
+    <t>Mark Williams</t>
+  </si>
+  <si>
+    <t>Robert Knapik</t>
+  </si>
+  <si>
+    <t>Richard Gurney</t>
+  </si>
+  <si>
+    <t>Honorable Chair</t>
+  </si>
+  <si>
+    <t>Glenn S. Frysinger</t>
+  </si>
+  <si>
+    <t>Mako Haruta</t>
+  </si>
+  <si>
+    <t>Jay Wang</t>
   </si>
   <si>
     <t>Matthew Griffiths</t>
   </si>
   <si>
-    <t>Gerald Darling</t>
-  </si>
-  <si>
-    <t>Paul Nakroshis</t>
-  </si>
-  <si>
-    <t>Candice Etson</t>
-  </si>
-  <si>
-    <t>Alica Chance</t>
+    <t>Leonard Kahn</t>
+  </si>
+  <si>
+    <t>Julie Ziffer</t>
+  </si>
+  <si>
+    <t>Yue Hu</t>
+  </si>
+  <si>
+    <t>Fred Ellis</t>
+  </si>
+  <si>
+    <t>James Boyle</t>
   </si>
   <si>
     <t>Fred Strauch</t>
   </si>
   <si>
-    <t>Kristina.A.Lynch@dartmouth.edu</t>
-  </si>
-  <si>
-    <t>checkelsky@mit.edu</t>
-  </si>
-  <si>
-    <t>smiths@mtholyoke.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ngugliucci@anselm.edu
-</t>
+    <t>michael.graf@bc.edu</t>
+  </si>
+  <si>
+    <t>vesna_mitrovic@brown.edu</t>
+  </si>
+  <si>
+    <t>James.W.LaBelle@dartmouth.edu</t>
+  </si>
+  <si>
+    <t>jstott@fairfield.edu</t>
+  </si>
+  <si>
+    <t>vafa@physics.harvard.edu</t>
+  </si>
+  <si>
+    <t>ashoori@mit.edu</t>
+  </si>
+  <si>
+    <t>idurham@anselm.edu</t>
+  </si>
+  <si>
+    <t>abrizard@smcvt.edu</t>
+  </si>
+  <si>
+    <t>nfortune@smith.edu</t>
   </si>
   <si>
     <t>wjohnson@suffolk.edu</t>
   </si>
   <si>
-    <t>frank.dudish@maine.edu</t>
-  </si>
-  <si>
-    <t>rpk101@wpi.edu</t>
-  </si>
-  <si>
-    <t>sarah.demers@yale.edu</t>
-  </si>
-  <si>
-    <t>TPARAMANATHAN@bridgew.edu</t>
-  </si>
-  <si>
-    <t>fell@brandeis.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Charles Thomas Hess</t>
-  </si>
-  <si>
-    <t>Greg Voth</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hess@maine.edu</t>
-  </si>
-  <si>
-    <t>gvoth@wesleyan.edu</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Inactive</t>
-  </si>
-  <si>
-    <t>Disbanded</t>
-  </si>
-  <si>
-    <t>Michael Graf</t>
-  </si>
-  <si>
-    <t>Vesna Mitrović​​</t>
-  </si>
-  <si>
-    <t>James LaBelle</t>
-  </si>
-  <si>
-    <t>Professor Brother Jonathan Stott, S.J.</t>
-  </si>
-  <si>
-    <t>Cumrun Vafa</t>
-  </si>
-  <si>
-    <t>Raymond Ashoori</t>
-  </si>
-  <si>
-    <t>Ian Durham</t>
-  </si>
-  <si>
-    <t>Alain Brizard</t>
-  </si>
-  <si>
-    <t>Nathanael Fortune</t>
-  </si>
-  <si>
-    <t>Barbara Walden</t>
-  </si>
-  <si>
-    <t>Lawrence Ford</t>
-  </si>
-  <si>
-    <t>John Thompson</t>
-  </si>
-  <si>
-    <t>Rahul Kulkarni</t>
-  </si>
-  <si>
-    <t>Arthur Mittler</t>
-  </si>
-  <si>
-    <t>Per Berglund</t>
-  </si>
-  <si>
-    <t>Randall Headrick</t>
-  </si>
-  <si>
-    <t>Doug Petkie</t>
-  </si>
-  <si>
-    <t>Karsten Heeger</t>
-  </si>
-  <si>
-    <t>David Hanneke</t>
-  </si>
-  <si>
-    <t>Andrei Ruckenstein</t>
-  </si>
-  <si>
-    <t>Tom Kling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kebra Ward </t>
-  </si>
-  <si>
-    <t>Seth Ashman</t>
-  </si>
-  <si>
-    <t>George Gibson</t>
-  </si>
-  <si>
-    <t>Anthony Dinsmore</t>
-  </si>
-  <si>
-    <t>John Michael Collins</t>
-  </si>
-  <si>
-    <t>Travis Gould</t>
-  </si>
-  <si>
-    <t>Steve Naculich</t>
-  </si>
-  <si>
-    <t>Jane' Kondev</t>
-  </si>
-  <si>
-    <t>Peter LeMaire</t>
-  </si>
-  <si>
-    <t>Arshad Kudrolli</t>
-  </si>
-  <si>
-    <t>Tom Narita</t>
-  </si>
-  <si>
-    <t>Pierre-Richard Cornely</t>
-  </si>
-  <si>
-    <t>Steven Harfenist</t>
-  </si>
-  <si>
-    <t>Sara Salimbeni</t>
-  </si>
-  <si>
-    <t>Craig Looney</t>
-  </si>
-  <si>
-    <t>Anne Goodsell</t>
-  </si>
-  <si>
-    <t>Mark Williams</t>
-  </si>
-  <si>
-    <t>Robert Knapik</t>
-  </si>
-  <si>
-    <t>Richard Gurney</t>
-  </si>
-  <si>
-    <t>Honorable Chair</t>
-  </si>
-  <si>
-    <t>Glenn S. Frysinger</t>
-  </si>
-  <si>
-    <t>Mako Haruta</t>
-  </si>
-  <si>
-    <t>Jay Wang</t>
-  </si>
-  <si>
-    <t>Leonard Kahn</t>
-  </si>
-  <si>
-    <t>Julie Ziffer</t>
-  </si>
-  <si>
-    <t>Yue Hu</t>
-  </si>
-  <si>
-    <t>Fred Ellis</t>
-  </si>
-  <si>
-    <t>James Boyle</t>
-  </si>
-  <si>
-    <t>michael.graf@bc.edu</t>
-  </si>
-  <si>
-    <t>vesna_mitrovic@brown.edu</t>
-  </si>
-  <si>
-    <t>James.W.LaBelle@dartmouth.edu</t>
-  </si>
-  <si>
-    <t>jstott@fairfield.edu</t>
-  </si>
-  <si>
-    <t>vafa@physics.harvard.edu</t>
-  </si>
-  <si>
-    <t>ashoori@mit.edu</t>
-  </si>
-  <si>
-    <t>idurham@anselm.edu</t>
-  </si>
-  <si>
-    <t>abrizard@smcvt.edu</t>
-  </si>
-  <si>
-    <t>nfortune@smith.edu</t>
-  </si>
-  <si>
     <t>barbara.walden@trincoll.edu</t>
   </si>
   <si>
@@ -1996,85 +1918,28 @@
     <t>University of Massachusetts Dartmouth</t>
   </si>
   <si>
-    <t>Zara Yu</t>
-  </si>
-  <si>
-    <t>Co-President: Latika Joshi</t>
-  </si>
-  <si>
-    <t>Mallika Sinha</t>
+    <t>Katerina Donahue</t>
+  </si>
+  <si>
+    <t>Annabelle Niblet</t>
+  </si>
+  <si>
+    <t>Jorge Garcia Ponce</t>
+  </si>
+  <si>
+    <t>Hope Fu</t>
+  </si>
+  <si>
+    <t>Christian Vogt</t>
+  </si>
+  <si>
+    <t>Ash Messier</t>
+  </si>
+  <si>
+    <t>Noah Stiegler</t>
   </si>
   <si>
     <t>Ryan Corzo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syrena Prytko </t>
-  </si>
-  <si>
-    <t>Aaron Chizhik</t>
-  </si>
-  <si>
-    <t>Michael Frank</t>
-  </si>
-  <si>
-    <t>Meredith Loscar</t>
-  </si>
-  <si>
-    <t>Savanna Coffel; Iris Sung</t>
-  </si>
-  <si>
-    <t>Matthew Stearns</t>
-  </si>
-  <si>
-    <t>zarayu@mit.edu</t>
-  </si>
-  <si>
-    <t>joshi23l@mtholyoke.edu</t>
-  </si>
-  <si>
-    <t>mallika.sinha@tufts.edu</t>
-  </si>
-  <si>
-    <t>ryan.corzo@maine.edu</t>
-  </si>
-  <si>
-    <t>smprytko@wpi.edu</t>
-  </si>
-  <si>
-    <t>aaron.chizhik@yale.edu</t>
-  </si>
-  <si>
-    <t>michael.frank@uconn.edu</t>
-  </si>
-  <si>
-    <t>mloscar@umass.edu</t>
-  </si>
-  <si>
-    <t>isung@college.harvard.edu</t>
-  </si>
-  <si>
-    <t>mstearns1@umassd.edu</t>
-  </si>
-  <si>
-    <t>Katerina Donahue</t>
-  </si>
-  <si>
-    <t>Annabelle Niblet</t>
-  </si>
-  <si>
-    <t>Jorge Garcia Ponce</t>
-  </si>
-  <si>
-    <t>Hope Fu</t>
-  </si>
-  <si>
-    <t>Christian Vogt</t>
-  </si>
-  <si>
-    <t>Ash Messier</t>
-  </si>
-  <si>
-    <t>Noah Stiegler</t>
   </si>
   <si>
     <t>Patrick O'Keefe</t>
@@ -2138,6 +2003,9 @@
     <t>amessier@smith.edu</t>
   </si>
   <si>
+    <t>ryan.corzo@maine.edu</t>
+  </si>
+  <si>
     <t>Patrick_OKeefe2@student.uml.edu</t>
   </si>
   <si>
@@ -2211,6 +2079,9 @@
     <t>kpanebia@mit.edu</t>
   </si>
   <si>
+    <t>joshi23l@mtholyoke.edu</t>
+  </si>
+  <si>
     <t>ckombo@mail.smcvt.edu</t>
   </si>
   <si>
@@ -2395,6 +2266,9 @@
   </si>
   <si>
     <t>Jeremy.Elliott@uvm.edu</t>
+  </si>
+  <si>
+    <t>smprytko@wpi.edu</t>
   </si>
   <si>
     <t>Rose.Branson@yale.edu, Ethan.Martinez@yale.edu, Robin.Tsai@yale.edu, Ryan.Bose-Roy@yale.edu, David.Saunders@yale.edu, Ruthie.Gu@yale.edu, Maddi Brown@yale.edu, Lumisa.Bista@yale.edu, Misheal.Saah@yale.edu, Maddie.Butchko@yale.edu</t>
@@ -2984,15 +2858,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10"/>
+    <sheetView tabSelected="1" topLeftCell="P46" workbookViewId="0">
+      <selection activeCell="V83" sqref="V83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="33" max="33" width="44.1640625" customWidth="1"/>
-    <col min="34" max="34" width="53.5" customWidth="1"/>
-    <col min="35" max="35" width="49.5" customWidth="1"/>
+    <col min="22" max="22" width="43.33203125" customWidth="1"/>
+    <col min="23" max="23" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.2">
@@ -3211,12 +3084,6 @@
       <c r="U2" t="s">
         <v>443</v>
       </c>
-      <c r="V2" t="s">
-        <v>449</v>
-      </c>
-      <c r="W2" t="s">
-        <v>123</v>
-      </c>
       <c r="X2" t="s">
         <v>443</v>
       </c>
@@ -3224,52 +3091,52 @@
         <v>443</v>
       </c>
       <c r="Z2" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA2" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB2" t="s">
-        <v>506</v>
+        <v>476</v>
       </c>
       <c r="AC2" t="s">
-        <v>555</v>
+        <v>529</v>
       </c>
       <c r="AD2" t="s">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="AE2" t="s">
-        <v>629</v>
+        <v>604</v>
       </c>
       <c r="AG2" t="s">
         <v>51</v>
       </c>
       <c r="AJ2" t="s">
-        <v>676</v>
+        <v>631</v>
       </c>
       <c r="AK2" t="s">
+        <v>653</v>
+      </c>
+      <c r="AN2" t="s">
         <v>697</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
+        <v>713</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>729</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>739</v>
       </c>
-      <c r="AO2" t="s">
-        <v>755</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>771</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>781</v>
-      </c>
       <c r="AR2" t="s">
-        <v>791</v>
+        <v>750</v>
       </c>
       <c r="AS2">
         <v>2019</v>
       </c>
       <c r="AX2" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
@@ -3330,12 +3197,6 @@
       <c r="U3" t="s">
         <v>443</v>
       </c>
-      <c r="V3" t="s">
-        <v>385</v>
-      </c>
-      <c r="W3" t="s">
-        <v>419</v>
-      </c>
       <c r="X3" t="s">
         <v>443</v>
       </c>
@@ -3343,40 +3204,40 @@
         <v>443</v>
       </c>
       <c r="Z3" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA3" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB3" t="s">
-        <v>507</v>
+        <v>477</v>
       </c>
       <c r="AC3" t="s">
-        <v>556</v>
+        <v>530</v>
       </c>
       <c r="AD3" t="s">
-        <v>601</v>
+        <v>576</v>
       </c>
       <c r="AE3" t="s">
-        <v>630</v>
+        <v>605</v>
       </c>
       <c r="AG3" t="s">
         <v>52</v>
       </c>
       <c r="AR3" t="s">
-        <v>792</v>
+        <v>751</v>
       </c>
       <c r="AT3" t="s">
-        <v>805</v>
+        <v>764</v>
       </c>
       <c r="AW3" t="s">
-        <v>812</v>
+        <v>771</v>
       </c>
       <c r="AX3" t="s">
-        <v>817</v>
+        <v>776</v>
       </c>
       <c r="AY3" t="s">
-        <v>838</v>
+        <v>797</v>
       </c>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.2">
@@ -3431,12 +3292,6 @@
       <c r="U4" t="s">
         <v>443</v>
       </c>
-      <c r="V4" t="s">
-        <v>450</v>
-      </c>
-      <c r="W4" t="s">
-        <v>489</v>
-      </c>
       <c r="X4" t="s">
         <v>443</v>
       </c>
@@ -3444,25 +3299,25 @@
         <v>443</v>
       </c>
       <c r="AA4" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB4" t="s">
-        <v>508</v>
+        <v>478</v>
       </c>
       <c r="AC4" t="s">
-        <v>557</v>
+        <v>531</v>
       </c>
       <c r="AG4" t="s">
         <v>53</v>
       </c>
       <c r="AJ4" t="s">
-        <v>677</v>
+        <v>632</v>
       </c>
       <c r="AK4" t="s">
-        <v>698</v>
+        <v>654</v>
       </c>
       <c r="AX4" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY4">
         <v>2023</v>
@@ -3524,28 +3379,28 @@
         <v>421</v>
       </c>
       <c r="V5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="W5" t="s">
         <v>126</v>
       </c>
       <c r="Z5" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA5" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB5" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="AC5" t="s">
-        <v>558</v>
+        <v>532</v>
       </c>
       <c r="AD5" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="AE5" t="s">
-        <v>630</v>
+        <v>605</v>
       </c>
       <c r="AG5" t="s">
         <v>54</v>
@@ -3554,7 +3409,7 @@
         <v>2019</v>
       </c>
       <c r="AX5" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY5">
         <v>2023</v>
@@ -3609,47 +3464,41 @@
       <c r="U6" t="s">
         <v>443</v>
       </c>
-      <c r="V6" t="s">
-        <v>452</v>
-      </c>
-      <c r="W6" t="s">
-        <v>127</v>
-      </c>
       <c r="Z6" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA6" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB6" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="AC6" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
       <c r="AD6" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="AE6" t="s">
-        <v>631</v>
+        <v>606</v>
       </c>
       <c r="AG6" t="s">
         <v>55</v>
       </c>
       <c r="AJ6" t="s">
-        <v>678</v>
+        <v>633</v>
       </c>
       <c r="AK6" t="s">
-        <v>699</v>
+        <v>655</v>
       </c>
       <c r="AQ6" t="s">
-        <v>782</v>
+        <v>740</v>
       </c>
       <c r="AR6">
         <v>2012</v>
       </c>
       <c r="AX6" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY6">
         <v>2023</v>
@@ -3717,10 +3566,10 @@
         <v>446</v>
       </c>
       <c r="V7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="W7" t="s">
-        <v>490</v>
+        <v>461</v>
       </c>
       <c r="X7" t="s">
         <v>444</v>
@@ -3729,58 +3578,52 @@
         <v>446</v>
       </c>
       <c r="Z7" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA7" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB7" t="s">
-        <v>511</v>
+        <v>481</v>
       </c>
       <c r="AC7" t="s">
-        <v>560</v>
+        <v>534</v>
       </c>
       <c r="AD7" t="s">
-        <v>604</v>
+        <v>579</v>
       </c>
       <c r="AE7" t="s">
-        <v>632</v>
+        <v>607</v>
       </c>
       <c r="AG7" t="s">
         <v>56</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AJ7" t="s">
+        <v>634</v>
+      </c>
+      <c r="AK7" t="s">
         <v>656</v>
       </c>
-      <c r="AI7" t="s">
-        <v>666</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>679</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>700</v>
-      </c>
       <c r="AL7" t="s">
-        <v>712</v>
+        <v>669</v>
       </c>
       <c r="AM7" t="s">
-        <v>726</v>
+        <v>683</v>
       </c>
       <c r="AN7" t="s">
-        <v>740</v>
+        <v>698</v>
       </c>
       <c r="AO7" t="s">
-        <v>756</v>
+        <v>714</v>
       </c>
       <c r="AR7" t="s">
-        <v>793</v>
+        <v>752</v>
       </c>
       <c r="AS7">
         <v>2021</v>
       </c>
       <c r="AX7" t="s">
-        <v>818</v>
+        <v>777</v>
       </c>
       <c r="AY7">
         <v>2023</v>
@@ -3848,10 +3691,10 @@
         <v>443</v>
       </c>
       <c r="V8" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="W8" t="s">
-        <v>491</v>
+        <v>462</v>
       </c>
       <c r="X8" t="s">
         <v>443</v>
@@ -3860,10 +3703,10 @@
         <v>443</v>
       </c>
       <c r="Z8" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA8" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB8" t="s">
         <v>389</v>
@@ -3872,40 +3715,34 @@
         <v>423</v>
       </c>
       <c r="AD8" t="s">
-        <v>605</v>
+        <v>580</v>
       </c>
       <c r="AE8" t="s">
-        <v>633</v>
+        <v>608</v>
       </c>
       <c r="AG8" t="s">
         <v>57</v>
       </c>
-      <c r="AH8" t="s">
-        <v>657</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>667</v>
-      </c>
       <c r="AL8" t="s">
-        <v>713</v>
+        <v>670</v>
       </c>
       <c r="AM8" t="s">
-        <v>667</v>
+        <v>684</v>
       </c>
       <c r="AN8" t="s">
+        <v>699</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>715</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>730</v>
+      </c>
+      <c r="AQ8" t="s">
         <v>741</v>
       </c>
-      <c r="AO8" t="s">
-        <v>757</v>
-      </c>
-      <c r="AP8" t="s">
-        <v>772</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>783</v>
-      </c>
       <c r="AS8" t="s">
-        <v>802</v>
+        <v>761</v>
       </c>
       <c r="AY8">
         <v>2023</v>
@@ -3970,46 +3807,46 @@
         <v>390</v>
       </c>
       <c r="W9" t="s">
-        <v>492</v>
+        <v>424</v>
       </c>
       <c r="Z9" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA9" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB9" t="s">
-        <v>512</v>
+        <v>482</v>
       </c>
       <c r="AC9" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
       <c r="AD9" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="AE9" t="s">
-        <v>630</v>
+        <v>605</v>
       </c>
       <c r="AG9" t="s">
         <v>58</v>
       </c>
       <c r="AR9" t="s">
-        <v>792</v>
+        <v>751</v>
       </c>
       <c r="AS9">
         <v>2022</v>
       </c>
       <c r="AU9" t="s">
-        <v>809</v>
+        <v>768</v>
       </c>
       <c r="AW9" t="s">
-        <v>813</v>
+        <v>772</v>
       </c>
       <c r="AX9" t="s">
-        <v>819</v>
+        <v>778</v>
       </c>
       <c r="AY9" t="s">
-        <v>839</v>
+        <v>798</v>
       </c>
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.2">
@@ -4067,56 +3904,50 @@
       <c r="S10" t="s">
         <v>425</v>
       </c>
-      <c r="V10" t="s">
-        <v>455</v>
-      </c>
-      <c r="W10" t="s">
-        <v>425</v>
-      </c>
       <c r="Z10" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA10" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB10" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
       <c r="AC10" t="s">
-        <v>562</v>
+        <v>536</v>
       </c>
       <c r="AD10" t="s">
-        <v>607</v>
+        <v>582</v>
       </c>
       <c r="AE10" t="s">
-        <v>634</v>
+        <v>609</v>
       </c>
       <c r="AG10" t="s">
         <v>59</v>
       </c>
       <c r="AJ10" t="s">
-        <v>680</v>
+        <v>635</v>
       </c>
       <c r="AK10" t="s">
-        <v>701</v>
+        <v>657</v>
       </c>
       <c r="AL10" t="s">
-        <v>714</v>
+        <v>671</v>
       </c>
       <c r="AM10" t="s">
-        <v>727</v>
+        <v>685</v>
       </c>
       <c r="AN10" t="s">
-        <v>742</v>
+        <v>700</v>
       </c>
       <c r="AO10" t="s">
-        <v>758</v>
+        <v>716</v>
       </c>
       <c r="AR10">
         <v>2019</v>
       </c>
       <c r="AU10" t="s">
-        <v>810</v>
+        <v>769</v>
       </c>
       <c r="AY10">
         <v>2022</v>
@@ -4163,58 +3994,58 @@
         <v>6466</v>
       </c>
       <c r="V11" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="W11" t="s">
         <v>132</v>
       </c>
       <c r="Z11" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA11" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB11" t="s">
-        <v>514</v>
+        <v>484</v>
       </c>
       <c r="AC11" t="s">
-        <v>563</v>
+        <v>537</v>
       </c>
       <c r="AD11">
         <v>4135853797</v>
       </c>
       <c r="AE11" t="s">
-        <v>632</v>
+        <v>607</v>
       </c>
       <c r="AG11" t="s">
         <v>60</v>
       </c>
       <c r="AJ11" t="s">
-        <v>681</v>
+        <v>636</v>
       </c>
       <c r="AK11" t="s">
-        <v>702</v>
+        <v>658</v>
       </c>
       <c r="AL11" t="s">
-        <v>715</v>
+        <v>672</v>
       </c>
       <c r="AM11" t="s">
-        <v>728</v>
+        <v>686</v>
       </c>
       <c r="AN11" t="s">
-        <v>743</v>
+        <v>701</v>
       </c>
       <c r="AO11" t="s">
-        <v>759</v>
+        <v>717</v>
       </c>
       <c r="AR11">
         <v>2022</v>
       </c>
       <c r="AX11" t="s">
-        <v>820</v>
+        <v>779</v>
       </c>
       <c r="AY11" t="s">
-        <v>840</v>
+        <v>799</v>
       </c>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.2">
@@ -4278,12 +4109,6 @@
       <c r="U12" t="s">
         <v>443</v>
       </c>
-      <c r="V12" t="s">
-        <v>457</v>
-      </c>
-      <c r="W12" t="s">
-        <v>493</v>
-      </c>
       <c r="X12" t="s">
         <v>443</v>
       </c>
@@ -4291,43 +4116,43 @@
         <v>443</v>
       </c>
       <c r="Z12" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA12" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB12" t="s">
-        <v>457</v>
+        <v>485</v>
       </c>
       <c r="AC12" t="s">
-        <v>493</v>
+        <v>538</v>
       </c>
       <c r="AD12">
         <v>6175738013</v>
       </c>
       <c r="AE12" t="s">
-        <v>635</v>
+        <v>610</v>
       </c>
       <c r="AF12" t="s">
-        <v>649</v>
+        <v>624</v>
       </c>
       <c r="AG12" t="s">
         <v>61</v>
       </c>
       <c r="AR12" t="s">
-        <v>794</v>
+        <v>753</v>
       </c>
       <c r="AT12" t="s">
-        <v>806</v>
+        <v>765</v>
       </c>
       <c r="AU12" t="s">
-        <v>811</v>
+        <v>770</v>
       </c>
       <c r="AX12" t="s">
-        <v>821</v>
+        <v>780</v>
       </c>
       <c r="AY12" t="s">
-        <v>839</v>
+        <v>798</v>
       </c>
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.2">
@@ -4391,12 +4216,6 @@
       <c r="U13" t="s">
         <v>443</v>
       </c>
-      <c r="V13" t="s">
-        <v>393</v>
-      </c>
-      <c r="W13" t="s">
-        <v>427</v>
-      </c>
       <c r="X13" t="s">
         <v>443</v>
       </c>
@@ -4404,22 +4223,22 @@
         <v>443</v>
       </c>
       <c r="Z13" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA13" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB13" t="s">
-        <v>515</v>
+        <v>486</v>
       </c>
       <c r="AC13" t="s">
-        <v>564</v>
+        <v>539</v>
       </c>
       <c r="AD13" t="s">
-        <v>608</v>
+        <v>583</v>
       </c>
       <c r="AE13" t="s">
-        <v>636</v>
+        <v>611</v>
       </c>
       <c r="AG13" t="s">
         <v>62</v>
@@ -4428,10 +4247,10 @@
         <v>2012</v>
       </c>
       <c r="AX13" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY13" t="s">
-        <v>839</v>
+        <v>798</v>
       </c>
     </row>
     <row r="14" spans="1:51" x14ac:dyDescent="0.2">
@@ -4499,64 +4318,58 @@
         <v>443</v>
       </c>
       <c r="V14" t="s">
-        <v>394</v>
+        <v>453</v>
       </c>
       <c r="W14" t="s">
-        <v>428</v>
+        <v>463</v>
       </c>
       <c r="Z14" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA14" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB14" t="s">
-        <v>516</v>
+        <v>487</v>
       </c>
       <c r="AC14" t="s">
-        <v>565</v>
+        <v>540</v>
       </c>
       <c r="AG14" t="s">
         <v>63</v>
       </c>
-      <c r="AH14" t="s">
-        <v>658</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>668</v>
-      </c>
       <c r="AJ14" t="s">
-        <v>682</v>
+        <v>637</v>
       </c>
       <c r="AK14" t="s">
         <v>135</v>
       </c>
       <c r="AL14" t="s">
-        <v>716</v>
+        <v>673</v>
       </c>
       <c r="AM14" t="s">
-        <v>729</v>
+        <v>687</v>
       </c>
       <c r="AN14" t="s">
-        <v>744</v>
+        <v>702</v>
       </c>
       <c r="AO14" t="s">
-        <v>760</v>
+        <v>718</v>
       </c>
       <c r="AP14" t="s">
-        <v>773</v>
+        <v>731</v>
       </c>
       <c r="AQ14" t="s">
-        <v>784</v>
+        <v>742</v>
       </c>
       <c r="AS14" t="s">
-        <v>803</v>
+        <v>762</v>
       </c>
       <c r="AX14" t="s">
-        <v>822</v>
+        <v>781</v>
       </c>
       <c r="AY14" t="s">
-        <v>841</v>
+        <v>800</v>
       </c>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.2">
@@ -4621,67 +4434,61 @@
         <v>447</v>
       </c>
       <c r="V15" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="W15" t="s">
-        <v>494</v>
+        <v>464</v>
       </c>
       <c r="X15" t="s">
-        <v>499</v>
+        <v>469</v>
       </c>
       <c r="Y15" t="s">
-        <v>501</v>
+        <v>471</v>
       </c>
       <c r="Z15" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA15" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB15" t="s">
-        <v>517</v>
+        <v>488</v>
       </c>
       <c r="AC15" t="s">
-        <v>566</v>
+        <v>541</v>
       </c>
       <c r="AD15" t="s">
-        <v>609</v>
+        <v>584</v>
       </c>
       <c r="AE15" t="s">
-        <v>637</v>
+        <v>612</v>
       </c>
       <c r="AF15" t="s">
-        <v>650</v>
+        <v>625</v>
       </c>
       <c r="AG15" t="s">
         <v>64</v>
       </c>
-      <c r="AH15" t="s">
+      <c r="AJ15" t="s">
+        <v>638</v>
+      </c>
+      <c r="AK15" t="s">
         <v>659</v>
       </c>
-      <c r="AI15" t="s">
-        <v>669</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>659</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>669</v>
-      </c>
       <c r="AL15" t="s">
-        <v>717</v>
+        <v>674</v>
       </c>
       <c r="AM15" t="s">
-        <v>730</v>
+        <v>688</v>
       </c>
       <c r="AN15" t="s">
-        <v>745</v>
+        <v>703</v>
       </c>
       <c r="AO15" t="s">
-        <v>761</v>
+        <v>719</v>
       </c>
       <c r="AR15" t="s">
-        <v>795</v>
+        <v>754</v>
       </c>
       <c r="AS15">
         <v>2018</v>
@@ -4690,13 +4497,13 @@
         <v>2017</v>
       </c>
       <c r="AW15" t="s">
-        <v>814</v>
+        <v>773</v>
       </c>
       <c r="AX15" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY15" t="s">
-        <v>842</v>
+        <v>801</v>
       </c>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.2">
@@ -4757,41 +4564,35 @@
       <c r="U16" t="s">
         <v>443</v>
       </c>
-      <c r="V16" t="s">
-        <v>459</v>
-      </c>
-      <c r="W16" t="s">
-        <v>137</v>
-      </c>
       <c r="Y16" t="s">
         <v>443</v>
       </c>
       <c r="Z16" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA16" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB16" t="s">
-        <v>518</v>
+        <v>489</v>
       </c>
       <c r="AC16" t="s">
-        <v>567</v>
+        <v>542</v>
       </c>
       <c r="AD16" t="s">
-        <v>610</v>
+        <v>585</v>
       </c>
       <c r="AG16" t="s">
         <v>65</v>
       </c>
       <c r="AR16" t="s">
-        <v>792</v>
+        <v>751</v>
       </c>
       <c r="AT16" t="s">
-        <v>807</v>
+        <v>766</v>
       </c>
       <c r="AY16" t="s">
-        <v>843</v>
+        <v>802</v>
       </c>
     </row>
     <row r="17" spans="1:51" x14ac:dyDescent="0.2">
@@ -4855,12 +4656,6 @@
       <c r="U17" t="s">
         <v>443</v>
       </c>
-      <c r="V17" t="s">
-        <v>397</v>
-      </c>
-      <c r="W17" t="s">
-        <v>431</v>
-      </c>
       <c r="X17" t="s">
         <v>443</v>
       </c>
@@ -4868,46 +4663,46 @@
         <v>443</v>
       </c>
       <c r="Z17" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA17" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB17" t="s">
-        <v>519</v>
+        <v>490</v>
       </c>
       <c r="AC17" t="s">
-        <v>568</v>
+        <v>543</v>
       </c>
       <c r="AD17" t="s">
-        <v>611</v>
+        <v>586</v>
       </c>
       <c r="AG17" t="s">
         <v>66</v>
       </c>
       <c r="AJ17" t="s">
-        <v>683</v>
+        <v>639</v>
       </c>
       <c r="AK17" t="s">
-        <v>703</v>
+        <v>660</v>
       </c>
       <c r="AL17" t="s">
-        <v>718</v>
+        <v>675</v>
       </c>
       <c r="AM17" t="s">
-        <v>731</v>
+        <v>689</v>
       </c>
       <c r="AN17" t="s">
-        <v>746</v>
+        <v>704</v>
       </c>
       <c r="AO17" t="s">
-        <v>762</v>
+        <v>720</v>
       </c>
       <c r="AP17" t="s">
-        <v>774</v>
+        <v>732</v>
       </c>
       <c r="AQ17" t="s">
-        <v>785</v>
+        <v>743</v>
       </c>
       <c r="AY17">
         <v>2023</v>
@@ -4974,12 +4769,6 @@
       <c r="U18" t="s">
         <v>443</v>
       </c>
-      <c r="V18" t="s">
-        <v>460</v>
-      </c>
-      <c r="W18" t="s">
-        <v>139</v>
-      </c>
       <c r="X18" t="s">
         <v>443</v>
       </c>
@@ -4987,19 +4776,19 @@
         <v>443</v>
       </c>
       <c r="Z18" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA18" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB18" t="s">
-        <v>520</v>
+        <v>491</v>
       </c>
       <c r="AC18" t="s">
-        <v>569</v>
+        <v>544</v>
       </c>
       <c r="AD18" t="s">
-        <v>612</v>
+        <v>587</v>
       </c>
       <c r="AG18" t="s">
         <v>67</v>
@@ -5008,7 +4797,7 @@
         <v>2012</v>
       </c>
       <c r="AX18" t="s">
-        <v>823</v>
+        <v>782</v>
       </c>
       <c r="AY18">
         <v>2023</v>
@@ -5075,12 +4864,6 @@
       <c r="U19" t="s">
         <v>443</v>
       </c>
-      <c r="V19" t="s">
-        <v>399</v>
-      </c>
-      <c r="W19" t="s">
-        <v>433</v>
-      </c>
       <c r="X19" t="s">
         <v>443</v>
       </c>
@@ -5088,52 +4871,52 @@
         <v>443</v>
       </c>
       <c r="Z19" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA19" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB19" t="s">
-        <v>521</v>
+        <v>492</v>
       </c>
       <c r="AC19" t="s">
-        <v>570</v>
+        <v>545</v>
       </c>
       <c r="AD19" t="s">
-        <v>613</v>
+        <v>588</v>
       </c>
       <c r="AG19" t="s">
-        <v>652</v>
+        <v>627</v>
       </c>
       <c r="AJ19" t="s">
-        <v>684</v>
+        <v>640</v>
       </c>
       <c r="AK19" t="s">
-        <v>704</v>
+        <v>661</v>
       </c>
       <c r="AL19" t="s">
-        <v>719</v>
+        <v>676</v>
       </c>
       <c r="AM19" t="s">
-        <v>732</v>
+        <v>690</v>
       </c>
       <c r="AN19" t="s">
-        <v>747</v>
+        <v>705</v>
       </c>
       <c r="AO19" t="s">
-        <v>763</v>
+        <v>721</v>
       </c>
       <c r="AP19" t="s">
-        <v>775</v>
+        <v>733</v>
       </c>
       <c r="AQ19" t="s">
-        <v>786</v>
+        <v>744</v>
       </c>
       <c r="AX19" t="s">
-        <v>824</v>
+        <v>783</v>
       </c>
       <c r="AY19" t="s">
-        <v>844</v>
+        <v>803</v>
       </c>
     </row>
     <row r="20" spans="1:51" x14ac:dyDescent="0.2">
@@ -5192,58 +4975,52 @@
         <v>434</v>
       </c>
       <c r="V20" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="W20" t="s">
-        <v>495</v>
+        <v>465</v>
       </c>
       <c r="Z20" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA20" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB20" t="s">
-        <v>522</v>
+        <v>493</v>
       </c>
       <c r="AC20" t="s">
-        <v>571</v>
+        <v>546</v>
       </c>
       <c r="AE20" t="s">
-        <v>638</v>
+        <v>613</v>
       </c>
       <c r="AG20" t="s">
         <v>69</v>
       </c>
-      <c r="AH20" t="s">
-        <v>660</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>670</v>
-      </c>
       <c r="AJ20" t="s">
-        <v>685</v>
+        <v>641</v>
       </c>
       <c r="AK20" t="s">
-        <v>705</v>
+        <v>662</v>
       </c>
       <c r="AL20" t="s">
-        <v>720</v>
+        <v>677</v>
       </c>
       <c r="AM20" t="s">
-        <v>733</v>
+        <v>691</v>
       </c>
       <c r="AN20" t="s">
-        <v>748</v>
+        <v>706</v>
       </c>
       <c r="AO20" t="s">
-        <v>764</v>
+        <v>722</v>
       </c>
       <c r="AP20" t="s">
-        <v>776</v>
+        <v>734</v>
       </c>
       <c r="AQ20" t="s">
-        <v>670</v>
+        <v>745</v>
       </c>
       <c r="AR20">
         <v>2019</v>
@@ -5252,10 +5029,10 @@
         <v>2014</v>
       </c>
       <c r="AX20" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY20" t="s">
-        <v>845</v>
+        <v>804</v>
       </c>
     </row>
     <row r="21" spans="1:51" x14ac:dyDescent="0.2">
@@ -5311,64 +5088,58 @@
         <v>435</v>
       </c>
       <c r="V21" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="W21" t="s">
-        <v>496</v>
+        <v>466</v>
       </c>
       <c r="Z21" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA21" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB21" t="s">
-        <v>523</v>
+        <v>494</v>
       </c>
       <c r="AC21" t="s">
-        <v>572</v>
+        <v>547</v>
       </c>
       <c r="AE21" t="s">
-        <v>639</v>
+        <v>614</v>
       </c>
       <c r="AG21" t="s">
         <v>70</v>
       </c>
-      <c r="AH21" t="s">
-        <v>661</v>
-      </c>
-      <c r="AI21" t="s">
-        <v>671</v>
-      </c>
       <c r="AJ21" t="s">
-        <v>686</v>
+        <v>642</v>
       </c>
       <c r="AK21" t="s">
-        <v>686</v>
+        <v>642</v>
       </c>
       <c r="AN21" t="s">
-        <v>749</v>
+        <v>707</v>
       </c>
       <c r="AO21" t="s">
-        <v>765</v>
+        <v>723</v>
       </c>
       <c r="AP21" t="s">
-        <v>777</v>
+        <v>735</v>
       </c>
       <c r="AQ21" t="s">
-        <v>787</v>
+        <v>746</v>
       </c>
       <c r="AR21" t="s">
-        <v>796</v>
+        <v>755</v>
       </c>
       <c r="AW21" t="s">
-        <v>812</v>
+        <v>771</v>
       </c>
       <c r="AX21" t="s">
-        <v>825</v>
+        <v>784</v>
       </c>
       <c r="AY21" t="s">
-        <v>846</v>
+        <v>805</v>
       </c>
     </row>
     <row r="22" spans="1:51" x14ac:dyDescent="0.2">
@@ -5408,23 +5179,17 @@
       <c r="O22">
         <v>181</v>
       </c>
-      <c r="V22" t="s">
-        <v>463</v>
-      </c>
-      <c r="W22" t="s">
-        <v>143</v>
-      </c>
       <c r="AB22" t="s">
-        <v>524</v>
+        <v>495</v>
       </c>
       <c r="AC22" t="s">
-        <v>573</v>
+        <v>548</v>
       </c>
       <c r="AD22" t="s">
-        <v>614</v>
+        <v>589</v>
       </c>
       <c r="AE22" t="s">
-        <v>640</v>
+        <v>615</v>
       </c>
       <c r="AG22" t="s">
         <v>71</v>
@@ -5494,62 +5259,56 @@
       <c r="U23" t="s">
         <v>443</v>
       </c>
-      <c r="V23" t="s">
-        <v>464</v>
-      </c>
-      <c r="W23" t="s">
-        <v>144</v>
-      </c>
       <c r="Z23" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA23" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB23" t="s">
-        <v>525</v>
+        <v>496</v>
       </c>
       <c r="AC23" t="s">
-        <v>574</v>
+        <v>549</v>
       </c>
       <c r="AD23" t="s">
-        <v>615</v>
+        <v>590</v>
       </c>
       <c r="AE23" t="s">
-        <v>641</v>
+        <v>616</v>
       </c>
       <c r="AG23" t="s">
         <v>72</v>
       </c>
       <c r="AJ23" t="s">
-        <v>687</v>
+        <v>643</v>
       </c>
       <c r="AK23" t="s">
-        <v>706</v>
+        <v>663</v>
       </c>
       <c r="AL23" t="s">
-        <v>721</v>
+        <v>678</v>
       </c>
       <c r="AM23" t="s">
-        <v>734</v>
+        <v>692</v>
       </c>
       <c r="AN23" t="s">
-        <v>750</v>
+        <v>708</v>
       </c>
       <c r="AO23" t="s">
-        <v>766</v>
+        <v>724</v>
       </c>
       <c r="AP23" t="s">
-        <v>778</v>
+        <v>736</v>
       </c>
       <c r="AQ23" t="s">
-        <v>788</v>
+        <v>747</v>
       </c>
       <c r="AR23" t="s">
-        <v>797</v>
+        <v>756</v>
       </c>
       <c r="AX23" t="s">
-        <v>826</v>
+        <v>785</v>
       </c>
     </row>
     <row r="24" spans="1:51" x14ac:dyDescent="0.2">
@@ -5598,53 +5357,47 @@
       <c r="U24" t="s">
         <v>443</v>
       </c>
-      <c r="V24" t="s">
-        <v>465</v>
-      </c>
-      <c r="W24" t="s">
+      <c r="Z24" t="s">
+        <v>473</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>473</v>
+      </c>
+      <c r="AB24" t="s">
         <v>497</v>
       </c>
-      <c r="Z24" t="s">
-        <v>503</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>503</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>526</v>
-      </c>
       <c r="AC24" t="s">
-        <v>575</v>
+        <v>550</v>
       </c>
       <c r="AD24" t="s">
-        <v>616</v>
+        <v>591</v>
       </c>
       <c r="AG24" t="s">
-        <v>653</v>
+        <v>628</v>
       </c>
       <c r="AJ24" t="s">
-        <v>688</v>
+        <v>644</v>
       </c>
       <c r="AK24" t="s">
-        <v>707</v>
+        <v>664</v>
       </c>
       <c r="AL24" t="s">
-        <v>722</v>
+        <v>679</v>
       </c>
       <c r="AM24" t="s">
-        <v>735</v>
+        <v>693</v>
       </c>
       <c r="AN24" t="s">
-        <v>751</v>
+        <v>709</v>
       </c>
       <c r="AO24" t="s">
-        <v>767</v>
+        <v>725</v>
       </c>
       <c r="AR24">
         <v>2019</v>
       </c>
       <c r="AY24" t="s">
-        <v>847</v>
+        <v>806</v>
       </c>
     </row>
     <row r="25" spans="1:51" x14ac:dyDescent="0.2">
@@ -5708,47 +5461,41 @@
       <c r="U25" t="s">
         <v>443</v>
       </c>
-      <c r="V25" t="s">
-        <v>466</v>
-      </c>
-      <c r="W25" t="s">
-        <v>436</v>
-      </c>
       <c r="Z25" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA25" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB25" t="s">
-        <v>527</v>
+        <v>498</v>
       </c>
       <c r="AC25" t="s">
-        <v>576</v>
+        <v>551</v>
       </c>
       <c r="AD25" t="s">
-        <v>617</v>
+        <v>592</v>
       </c>
       <c r="AG25" t="s">
         <v>74</v>
       </c>
       <c r="AJ25" t="s">
-        <v>689</v>
+        <v>645</v>
       </c>
       <c r="AK25" t="s">
-        <v>708</v>
+        <v>665</v>
       </c>
       <c r="AL25" t="s">
-        <v>723</v>
+        <v>680</v>
       </c>
       <c r="AM25" t="s">
-        <v>736</v>
+        <v>694</v>
       </c>
       <c r="AN25" t="s">
-        <v>752</v>
+        <v>710</v>
       </c>
       <c r="AO25" t="s">
-        <v>768</v>
+        <v>726</v>
       </c>
       <c r="AR25">
         <v>2019</v>
@@ -5757,7 +5504,7 @@
         <v>2012</v>
       </c>
       <c r="AY25" t="s">
-        <v>848</v>
+        <v>807</v>
       </c>
     </row>
     <row r="26" spans="1:51" x14ac:dyDescent="0.2">
@@ -5821,12 +5568,6 @@
       <c r="U26" t="s">
         <v>443</v>
       </c>
-      <c r="V26" t="s">
-        <v>467</v>
-      </c>
-      <c r="W26" t="s">
-        <v>437</v>
-      </c>
       <c r="X26" t="s">
         <v>443</v>
       </c>
@@ -5834,28 +5575,28 @@
         <v>443</v>
       </c>
       <c r="Z26" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA26" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB26" t="s">
-        <v>528</v>
+        <v>499</v>
       </c>
       <c r="AC26" t="s">
-        <v>577</v>
+        <v>552</v>
       </c>
       <c r="AG26" t="s">
         <v>75</v>
       </c>
       <c r="AJ26" t="s">
-        <v>690</v>
+        <v>646</v>
       </c>
       <c r="AK26" t="s">
-        <v>709</v>
+        <v>666</v>
       </c>
       <c r="AX26" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.2">
@@ -5920,7 +5661,7 @@
         <v>443</v>
       </c>
       <c r="V27" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="W27" t="s">
         <v>148</v>
@@ -5932,40 +5673,34 @@
         <v>443</v>
       </c>
       <c r="Z27" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA27" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB27" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="AC27" t="s">
-        <v>578</v>
+        <v>553</v>
       </c>
       <c r="AD27" t="s">
-        <v>618</v>
+        <v>593</v>
       </c>
       <c r="AE27" t="s">
-        <v>642</v>
+        <v>617</v>
       </c>
       <c r="AG27" t="s">
         <v>76</v>
       </c>
-      <c r="AH27" t="s">
-        <v>662</v>
-      </c>
-      <c r="AI27" t="s">
-        <v>672</v>
-      </c>
       <c r="AR27" t="s">
-        <v>797</v>
+        <v>756</v>
       </c>
       <c r="AX27" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY27" t="s">
-        <v>849</v>
+        <v>808</v>
       </c>
     </row>
     <row r="28" spans="1:51" x14ac:dyDescent="0.2">
@@ -6015,10 +5750,10 @@
         <v>443</v>
       </c>
       <c r="V28" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="W28" t="s">
-        <v>149</v>
+        <v>467</v>
       </c>
       <c r="X28" t="s">
         <v>443</v>
@@ -6027,31 +5762,25 @@
         <v>443</v>
       </c>
       <c r="Z28" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA28" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB28" t="s">
-        <v>530</v>
+        <v>501</v>
       </c>
       <c r="AC28" t="s">
-        <v>579</v>
+        <v>554</v>
       </c>
       <c r="AD28" t="s">
-        <v>619</v>
+        <v>594</v>
       </c>
       <c r="AG28" t="s">
         <v>77</v>
       </c>
-      <c r="AH28" t="s">
-        <v>663</v>
-      </c>
-      <c r="AI28" t="s">
-        <v>673</v>
-      </c>
       <c r="AY28" t="s">
-        <v>850</v>
+        <v>809</v>
       </c>
     </row>
     <row r="29" spans="1:51" x14ac:dyDescent="0.2">
@@ -6098,55 +5827,55 @@
         <v>8145</v>
       </c>
       <c r="Z29" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA29" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB29" t="s">
-        <v>531</v>
+        <v>502</v>
       </c>
       <c r="AC29" t="s">
-        <v>580</v>
+        <v>555</v>
       </c>
       <c r="AD29" t="s">
-        <v>620</v>
+        <v>595</v>
       </c>
       <c r="AE29" t="s">
-        <v>643</v>
+        <v>618</v>
       </c>
       <c r="AF29" t="s">
-        <v>651</v>
+        <v>626</v>
       </c>
       <c r="AG29" t="s">
         <v>78</v>
       </c>
       <c r="AJ29" t="s">
-        <v>691</v>
+        <v>647</v>
       </c>
       <c r="AK29" t="s">
-        <v>710</v>
+        <v>667</v>
       </c>
       <c r="AL29" t="s">
-        <v>724</v>
+        <v>681</v>
       </c>
       <c r="AM29" t="s">
+        <v>695</v>
+      </c>
+      <c r="AN29" t="s">
+        <v>711</v>
+      </c>
+      <c r="AO29" t="s">
+        <v>727</v>
+      </c>
+      <c r="AP29" t="s">
         <v>737</v>
       </c>
-      <c r="AN29" t="s">
-        <v>753</v>
-      </c>
-      <c r="AO29" t="s">
-        <v>769</v>
-      </c>
-      <c r="AP29" t="s">
-        <v>779</v>
-      </c>
       <c r="AQ29" t="s">
-        <v>789</v>
+        <v>748</v>
       </c>
       <c r="AX29" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
     </row>
     <row r="30" spans="1:51" x14ac:dyDescent="0.2">
@@ -6172,13 +5901,13 @@
         <v>167</v>
       </c>
       <c r="Z30" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG30" t="s">
         <v>79</v>
       </c>
       <c r="AX30" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
     </row>
     <row r="31" spans="1:51" x14ac:dyDescent="0.2">
@@ -6204,13 +5933,13 @@
         <v>307</v>
       </c>
       <c r="Z31" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG31" t="s">
         <v>80</v>
       </c>
       <c r="AX31" t="s">
-        <v>825</v>
+        <v>784</v>
       </c>
     </row>
     <row r="32" spans="1:51" x14ac:dyDescent="0.2">
@@ -6256,29 +5985,23 @@
       <c r="O32">
         <v>445</v>
       </c>
-      <c r="V32" t="s">
-        <v>470</v>
-      </c>
-      <c r="W32" t="s">
-        <v>151</v>
-      </c>
       <c r="Z32" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB32" t="s">
-        <v>532</v>
+        <v>503</v>
       </c>
       <c r="AC32" t="s">
-        <v>581</v>
+        <v>556</v>
       </c>
       <c r="AD32" t="s">
-        <v>621</v>
+        <v>596</v>
       </c>
       <c r="AG32" t="s">
         <v>81</v>
       </c>
       <c r="AX32" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
     </row>
     <row r="33" spans="1:51" x14ac:dyDescent="0.2">
@@ -6301,7 +6024,7 @@
         <v>463</v>
       </c>
       <c r="Z33" t="s">
-        <v>505</v>
+        <v>475</v>
       </c>
       <c r="AG33" t="s">
         <v>82</v>
@@ -6333,16 +6056,16 @@
         <v>41738</v>
       </c>
       <c r="Z34" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG34" t="s">
         <v>83</v>
       </c>
       <c r="AX34" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY34" t="s">
-        <v>808</v>
+        <v>767</v>
       </c>
     </row>
     <row r="35" spans="1:51" x14ac:dyDescent="0.2">
@@ -6388,41 +6111,35 @@
       <c r="O35">
         <v>634</v>
       </c>
-      <c r="V35" t="s">
-        <v>471</v>
-      </c>
-      <c r="W35" t="s">
-        <v>152</v>
-      </c>
       <c r="Z35" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB35" t="s">
-        <v>533</v>
+        <v>504</v>
       </c>
       <c r="AC35" t="s">
-        <v>582</v>
+        <v>557</v>
       </c>
       <c r="AD35" t="s">
-        <v>622</v>
+        <v>597</v>
       </c>
       <c r="AG35" t="s">
         <v>84</v>
       </c>
       <c r="AR35" t="s">
-        <v>796</v>
+        <v>755</v>
       </c>
       <c r="AS35" t="s">
-        <v>804</v>
+        <v>763</v>
       </c>
       <c r="AW35" t="s">
-        <v>815</v>
+        <v>774</v>
       </c>
       <c r="AX35" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY35" t="s">
-        <v>806</v>
+        <v>765</v>
       </c>
     </row>
     <row r="36" spans="1:51" x14ac:dyDescent="0.2">
@@ -6471,12 +6188,6 @@
       <c r="U36" t="s">
         <v>443</v>
       </c>
-      <c r="V36" t="s">
-        <v>472</v>
-      </c>
-      <c r="W36" t="s">
-        <v>498</v>
-      </c>
       <c r="X36" t="s">
         <v>443</v>
       </c>
@@ -6484,22 +6195,22 @@
         <v>443</v>
       </c>
       <c r="Z36" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA36" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB36" t="s">
-        <v>534</v>
+        <v>505</v>
       </c>
       <c r="AC36" t="s">
-        <v>583</v>
+        <v>558</v>
       </c>
       <c r="AG36" t="s">
         <v>85</v>
       </c>
       <c r="AX36" t="s">
-        <v>827</v>
+        <v>786</v>
       </c>
     </row>
     <row r="37" spans="1:51" x14ac:dyDescent="0.2">
@@ -6522,7 +6233,7 @@
         <v>959</v>
       </c>
       <c r="Z37" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AG37" t="s">
         <v>86</v>
@@ -6592,12 +6303,6 @@
       <c r="U38" t="s">
         <v>443</v>
       </c>
-      <c r="V38" t="s">
-        <v>406</v>
-      </c>
-      <c r="W38" t="s">
-        <v>154</v>
-      </c>
       <c r="X38" t="s">
         <v>443</v>
       </c>
@@ -6605,28 +6310,28 @@
         <v>443</v>
       </c>
       <c r="Z38" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA38" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB38" t="s">
-        <v>535</v>
+        <v>506</v>
       </c>
       <c r="AC38" t="s">
-        <v>584</v>
+        <v>559</v>
       </c>
       <c r="AD38" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="AG38" t="s">
         <v>87</v>
       </c>
       <c r="AR38" t="s">
-        <v>798</v>
+        <v>757</v>
       </c>
       <c r="AX38" t="s">
-        <v>828</v>
+        <v>787</v>
       </c>
     </row>
     <row r="39" spans="1:51" x14ac:dyDescent="0.2">
@@ -6690,12 +6395,6 @@
       <c r="U39" t="s">
         <v>443</v>
       </c>
-      <c r="V39" t="s">
-        <v>473</v>
-      </c>
-      <c r="W39" t="s">
-        <v>155</v>
-      </c>
       <c r="X39" t="s">
         <v>443</v>
       </c>
@@ -6703,25 +6402,25 @@
         <v>443</v>
       </c>
       <c r="Z39" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA39" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB39" t="s">
-        <v>536</v>
+        <v>507</v>
       </c>
       <c r="AC39" t="s">
-        <v>585</v>
+        <v>560</v>
       </c>
       <c r="AD39" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="AG39" t="s">
         <v>88</v>
       </c>
       <c r="AR39" t="s">
-        <v>799</v>
+        <v>758</v>
       </c>
     </row>
     <row r="40" spans="1:51" x14ac:dyDescent="0.2">
@@ -6779,17 +6478,11 @@
       <c r="S40" t="s">
         <v>440</v>
       </c>
-      <c r="V40" t="s">
-        <v>408</v>
-      </c>
-      <c r="W40" t="s">
-        <v>440</v>
-      </c>
       <c r="Z40" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA40" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB40" t="s">
         <v>408</v>
@@ -6801,10 +6494,10 @@
         <v>89</v>
       </c>
       <c r="AX40" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="AY40" t="s">
-        <v>849</v>
+        <v>808</v>
       </c>
     </row>
     <row r="41" spans="1:51" x14ac:dyDescent="0.2">
@@ -6868,12 +6561,6 @@
       <c r="U41" t="s">
         <v>443</v>
       </c>
-      <c r="V41" t="s">
-        <v>409</v>
-      </c>
-      <c r="W41" t="s">
-        <v>157</v>
-      </c>
       <c r="X41" t="s">
         <v>443</v>
       </c>
@@ -6881,25 +6568,25 @@
         <v>443</v>
       </c>
       <c r="Z41" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA41" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB41" t="s">
-        <v>537</v>
+        <v>508</v>
       </c>
       <c r="AC41" t="s">
         <v>157</v>
       </c>
       <c r="AD41" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="AG41" t="s">
         <v>90</v>
       </c>
       <c r="AJ41" t="s">
-        <v>692</v>
+        <v>648</v>
       </c>
     </row>
     <row r="42" spans="1:51" x14ac:dyDescent="0.2">
@@ -6963,12 +6650,6 @@
       <c r="U42" t="s">
         <v>443</v>
       </c>
-      <c r="V42" t="s">
-        <v>474</v>
-      </c>
-      <c r="W42" t="s">
-        <v>158</v>
-      </c>
       <c r="X42" t="s">
         <v>443</v>
       </c>
@@ -6976,10 +6657,10 @@
         <v>443</v>
       </c>
       <c r="Z42" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA42" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB42" t="s">
         <v>410</v>
@@ -6988,13 +6669,13 @@
         <v>441</v>
       </c>
       <c r="AD42" t="s">
-        <v>623</v>
+        <v>598</v>
       </c>
       <c r="AG42" t="s">
         <v>91</v>
       </c>
       <c r="AX42" t="s">
-        <v>826</v>
+        <v>785</v>
       </c>
     </row>
     <row r="43" spans="1:51" x14ac:dyDescent="0.2">
@@ -7046,12 +6727,6 @@
       <c r="U43" t="s">
         <v>443</v>
       </c>
-      <c r="V43" t="s">
-        <v>475</v>
-      </c>
-      <c r="W43" t="s">
-        <v>159</v>
-      </c>
       <c r="X43" t="s">
         <v>443</v>
       </c>
@@ -7059,19 +6734,19 @@
         <v>443</v>
       </c>
       <c r="Z43" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB43" t="s">
-        <v>538</v>
+        <v>509</v>
       </c>
       <c r="AC43" t="s">
         <v>159</v>
       </c>
       <c r="AD43" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="AG43" t="s">
-        <v>654</v>
+        <v>629</v>
       </c>
     </row>
     <row r="44" spans="1:51" x14ac:dyDescent="0.2">
@@ -7097,7 +6772,7 @@
         <v>1803</v>
       </c>
       <c r="Z44" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG44" t="s">
         <v>93</v>
@@ -7126,7 +6801,7 @@
         <v>1963</v>
       </c>
       <c r="Z45" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AG45" t="s">
         <v>94</v>
@@ -7158,13 +6833,13 @@
         <v>2445</v>
       </c>
       <c r="Z46" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AG46" t="s">
         <v>95</v>
       </c>
       <c r="AY46" t="s">
-        <v>851</v>
+        <v>810</v>
       </c>
     </row>
     <row r="47" spans="1:51" x14ac:dyDescent="0.2">
@@ -7225,12 +6900,6 @@
       <c r="U47" t="s">
         <v>443</v>
       </c>
-      <c r="V47" t="s">
-        <v>476</v>
-      </c>
-      <c r="W47" t="s">
-        <v>160</v>
-      </c>
       <c r="X47" t="s">
         <v>443</v>
       </c>
@@ -7238,34 +6907,34 @@
         <v>443</v>
       </c>
       <c r="Z47" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA47" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB47" t="s">
-        <v>476</v>
+        <v>510</v>
       </c>
       <c r="AC47" t="s">
         <v>160</v>
       </c>
       <c r="AD47" t="s">
-        <v>624</v>
+        <v>599</v>
       </c>
       <c r="AE47" t="s">
-        <v>644</v>
+        <v>619</v>
       </c>
       <c r="AG47" t="s">
         <v>96</v>
       </c>
       <c r="AJ47" t="s">
-        <v>693</v>
+        <v>649</v>
       </c>
       <c r="AX47" t="s">
-        <v>829</v>
+        <v>788</v>
       </c>
       <c r="AY47" t="s">
-        <v>852</v>
+        <v>811</v>
       </c>
     </row>
     <row r="48" spans="1:51" x14ac:dyDescent="0.2">
@@ -7323,12 +6992,6 @@
       <c r="U48" t="s">
         <v>443</v>
       </c>
-      <c r="V48" t="s">
-        <v>477</v>
-      </c>
-      <c r="W48" t="s">
-        <v>161</v>
-      </c>
       <c r="X48" t="s">
         <v>443</v>
       </c>
@@ -7336,25 +6999,25 @@
         <v>443</v>
       </c>
       <c r="AA48" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB48" t="s">
-        <v>539</v>
+        <v>511</v>
       </c>
       <c r="AC48" t="s">
         <v>161</v>
       </c>
       <c r="AD48" t="s">
-        <v>625</v>
+        <v>600</v>
       </c>
       <c r="AG48" t="s">
         <v>97</v>
       </c>
       <c r="AX48" t="s">
-        <v>830</v>
+        <v>789</v>
       </c>
       <c r="AY48" t="s">
-        <v>849</v>
+        <v>808</v>
       </c>
     </row>
     <row r="49" spans="1:51" x14ac:dyDescent="0.2">
@@ -7388,23 +7051,23 @@
       <c r="O49">
         <v>4107</v>
       </c>
+      <c r="V49" t="s">
+        <v>459</v>
+      </c>
+      <c r="W49" t="s">
+        <v>127</v>
+      </c>
       <c r="Z49" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB49" t="s">
-        <v>540</v>
+        <v>512</v>
       </c>
       <c r="AC49" t="s">
-        <v>586</v>
+        <v>561</v>
       </c>
       <c r="AG49" t="s">
         <v>98</v>
-      </c>
-      <c r="AH49" t="s">
-        <v>664</v>
-      </c>
-      <c r="AI49" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="50" spans="1:51" x14ac:dyDescent="0.2">
@@ -7442,22 +7105,22 @@
         <v>4219</v>
       </c>
       <c r="Z50" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB50" t="s">
-        <v>541</v>
+        <v>513</v>
       </c>
       <c r="AC50" t="s">
-        <v>587</v>
+        <v>562</v>
       </c>
       <c r="AG50" t="s">
         <v>99</v>
       </c>
       <c r="AX50" t="s">
-        <v>831</v>
+        <v>790</v>
       </c>
       <c r="AY50" t="s">
-        <v>853</v>
+        <v>812</v>
       </c>
     </row>
     <row r="51" spans="1:51" x14ac:dyDescent="0.2">
@@ -7498,10 +7161,10 @@
         <v>4283</v>
       </c>
       <c r="Z51" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB51" t="s">
-        <v>542</v>
+        <v>514</v>
       </c>
       <c r="AC51" t="s">
         <v>162</v>
@@ -7571,12 +7234,6 @@
       <c r="U52" t="s">
         <v>448</v>
       </c>
-      <c r="V52" t="s">
-        <v>412</v>
-      </c>
-      <c r="W52" t="s">
-        <v>163</v>
-      </c>
       <c r="X52" t="s">
         <v>443</v>
       </c>
@@ -7584,19 +7241,19 @@
         <v>443</v>
       </c>
       <c r="Z52" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA52" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB52" t="s">
-        <v>543</v>
+        <v>515</v>
       </c>
       <c r="AC52" t="s">
-        <v>588</v>
+        <v>563</v>
       </c>
       <c r="AE52" t="s">
-        <v>645</v>
+        <v>620</v>
       </c>
       <c r="AG52" t="s">
         <v>101</v>
@@ -7605,10 +7262,10 @@
         <v>85.404166666666669</v>
       </c>
       <c r="AT52" t="s">
-        <v>808</v>
+        <v>767</v>
       </c>
       <c r="AX52" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
     </row>
     <row r="53" spans="1:51" x14ac:dyDescent="0.2">
@@ -7651,29 +7308,23 @@
       <c r="O53">
         <v>5008</v>
       </c>
-      <c r="V53" t="s">
-        <v>478</v>
-      </c>
-      <c r="W53" t="s">
-        <v>164</v>
-      </c>
       <c r="Z53" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB53" t="s">
-        <v>544</v>
+        <v>516</v>
       </c>
       <c r="AC53" t="s">
-        <v>589</v>
+        <v>564</v>
       </c>
       <c r="AG53" t="s">
         <v>102</v>
       </c>
       <c r="AJ53" t="s">
-        <v>694</v>
+        <v>650</v>
       </c>
       <c r="AX53" t="s">
-        <v>825</v>
+        <v>784</v>
       </c>
     </row>
     <row r="54" spans="1:51" x14ac:dyDescent="0.2">
@@ -7699,7 +7350,7 @@
         <v>5930</v>
       </c>
       <c r="Z54" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG54" t="s">
         <v>103</v>
@@ -7751,12 +7402,6 @@
       <c r="U55" t="s">
         <v>443</v>
       </c>
-      <c r="V55" t="s">
-        <v>479</v>
-      </c>
-      <c r="W55" t="s">
-        <v>165</v>
-      </c>
       <c r="X55" t="s">
         <v>443</v>
       </c>
@@ -7764,25 +7409,25 @@
         <v>443</v>
       </c>
       <c r="Z55" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA55" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB55" t="s">
-        <v>545</v>
+        <v>517</v>
       </c>
       <c r="AC55" t="s">
-        <v>590</v>
+        <v>565</v>
       </c>
       <c r="AE55" t="s">
-        <v>646</v>
+        <v>621</v>
       </c>
       <c r="AG55" t="s">
         <v>104</v>
       </c>
       <c r="AY55" t="s">
-        <v>854</v>
+        <v>813</v>
       </c>
     </row>
     <row r="56" spans="1:51" x14ac:dyDescent="0.2">
@@ -7808,13 +7453,13 @@
         <v>6562</v>
       </c>
       <c r="Z56" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG56" t="s">
         <v>105</v>
       </c>
       <c r="AY56" t="s">
-        <v>855</v>
+        <v>814</v>
       </c>
     </row>
     <row r="57" spans="1:51" x14ac:dyDescent="0.2">
@@ -7869,12 +7514,6 @@
       <c r="U57" t="s">
         <v>443</v>
       </c>
-      <c r="V57" t="s">
-        <v>413</v>
-      </c>
-      <c r="W57" t="s">
-        <v>166</v>
-      </c>
       <c r="X57" t="s">
         <v>443</v>
       </c>
@@ -7882,10 +7521,10 @@
         <v>443</v>
       </c>
       <c r="Z57" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA57" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB57" t="s">
         <v>413</v>
@@ -7897,10 +7536,10 @@
         <v>106</v>
       </c>
       <c r="AR57" t="s">
-        <v>800</v>
+        <v>759</v>
       </c>
       <c r="AX57" t="s">
-        <v>825</v>
+        <v>784</v>
       </c>
     </row>
     <row r="58" spans="1:51" x14ac:dyDescent="0.2">
@@ -7955,26 +7594,20 @@
       <c r="R58" t="s">
         <v>414</v>
       </c>
-      <c r="V58" t="s">
-        <v>480</v>
-      </c>
-      <c r="W58" t="s">
-        <v>167</v>
-      </c>
       <c r="Z58" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA58" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB58" t="s">
-        <v>546</v>
+        <v>518</v>
       </c>
       <c r="AC58" t="s">
-        <v>591</v>
+        <v>566</v>
       </c>
       <c r="AD58" t="s">
-        <v>591</v>
+        <v>566</v>
       </c>
       <c r="AG58" t="s">
         <v>107</v>
@@ -8026,12 +7659,6 @@
       <c r="U59" t="s">
         <v>443</v>
       </c>
-      <c r="V59" t="s">
-        <v>481</v>
-      </c>
-      <c r="W59" t="s">
-        <v>168</v>
-      </c>
       <c r="X59" t="s">
         <v>443</v>
       </c>
@@ -8039,28 +7666,28 @@
         <v>443</v>
       </c>
       <c r="Z59" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA59" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB59" t="s">
-        <v>547</v>
+        <v>519</v>
       </c>
       <c r="AC59" t="s">
-        <v>592</v>
+        <v>567</v>
       </c>
       <c r="AD59" t="s">
-        <v>626</v>
+        <v>601</v>
       </c>
       <c r="AG59" t="s">
         <v>108</v>
       </c>
       <c r="AX59" t="s">
-        <v>832</v>
+        <v>791</v>
       </c>
       <c r="AY59" t="s">
-        <v>849</v>
+        <v>808</v>
       </c>
     </row>
     <row r="60" spans="1:51" x14ac:dyDescent="0.2">
@@ -8107,16 +7734,16 @@
         <v>443</v>
       </c>
       <c r="Z60" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA60" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG60" t="s">
         <v>109</v>
       </c>
       <c r="AX60" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
     </row>
     <row r="61" spans="1:51" x14ac:dyDescent="0.2">
@@ -8165,12 +7792,6 @@
       <c r="U61" t="s">
         <v>443</v>
       </c>
-      <c r="V61" t="s">
-        <v>482</v>
-      </c>
-      <c r="W61" t="s">
-        <v>169</v>
-      </c>
       <c r="X61" t="s">
         <v>443</v>
       </c>
@@ -8178,25 +7799,25 @@
         <v>443</v>
       </c>
       <c r="Z61" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA61" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB61" t="s">
-        <v>548</v>
+        <v>520</v>
       </c>
       <c r="AC61" t="s">
-        <v>593</v>
+        <v>568</v>
       </c>
       <c r="AG61" t="s">
         <v>110</v>
       </c>
       <c r="AX61" t="s">
-        <v>833</v>
+        <v>792</v>
       </c>
       <c r="AY61" t="s">
-        <v>856</v>
+        <v>815</v>
       </c>
     </row>
     <row r="62" spans="1:51" x14ac:dyDescent="0.2">
@@ -8222,7 +7843,7 @@
         <v>3894</v>
       </c>
       <c r="Z62" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG62" t="s">
         <v>111</v>
@@ -8290,10 +7911,10 @@
         <v>443</v>
       </c>
       <c r="V63" t="s">
-        <v>415</v>
+        <v>460</v>
       </c>
       <c r="W63" t="s">
-        <v>170</v>
+        <v>468</v>
       </c>
       <c r="X63" t="s">
         <v>443</v>
@@ -8302,25 +7923,19 @@
         <v>443</v>
       </c>
       <c r="Z63" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA63" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB63" t="s">
-        <v>549</v>
+        <v>521</v>
       </c>
       <c r="AC63" t="s">
-        <v>594</v>
+        <v>569</v>
       </c>
       <c r="AG63" t="s">
-        <v>655</v>
-      </c>
-      <c r="AH63" t="s">
-        <v>665</v>
-      </c>
-      <c r="AI63" t="s">
-        <v>675</v>
+        <v>630</v>
       </c>
       <c r="AT63">
         <v>2013</v>
@@ -8372,12 +7987,6 @@
       <c r="U64" t="s">
         <v>443</v>
       </c>
-      <c r="V64" t="s">
-        <v>483</v>
-      </c>
-      <c r="W64" t="s">
-        <v>171</v>
-      </c>
       <c r="X64" t="s">
         <v>443</v>
       </c>
@@ -8385,28 +7994,28 @@
         <v>443</v>
       </c>
       <c r="Z64" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA64" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB64" t="s">
-        <v>483</v>
+        <v>522</v>
       </c>
       <c r="AC64" t="s">
         <v>171</v>
       </c>
       <c r="AD64" t="s">
-        <v>627</v>
+        <v>602</v>
       </c>
       <c r="AG64" t="s">
         <v>113</v>
       </c>
       <c r="AX64" t="s">
-        <v>834</v>
+        <v>793</v>
       </c>
       <c r="AY64" t="s">
-        <v>857</v>
+        <v>816</v>
       </c>
     </row>
     <row r="65" spans="1:51" x14ac:dyDescent="0.2">
@@ -8470,12 +8079,6 @@
       <c r="U65" t="s">
         <v>443</v>
       </c>
-      <c r="V65" t="s">
-        <v>416</v>
-      </c>
-      <c r="W65" t="s">
-        <v>172</v>
-      </c>
       <c r="X65" t="s">
         <v>443</v>
       </c>
@@ -8483,16 +8086,16 @@
         <v>443</v>
       </c>
       <c r="Z65" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AA65" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AB65" t="s">
-        <v>550</v>
+        <v>523</v>
       </c>
       <c r="AC65" t="s">
-        <v>595</v>
+        <v>570</v>
       </c>
       <c r="AG65" t="s">
         <v>114</v>
@@ -8501,7 +8104,7 @@
         <v>2019</v>
       </c>
       <c r="AX65" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
     </row>
     <row r="66" spans="1:51" x14ac:dyDescent="0.2">
@@ -8553,17 +8156,11 @@
       <c r="S66" t="s">
         <v>442</v>
       </c>
-      <c r="V66" t="s">
-        <v>484</v>
-      </c>
-      <c r="W66" t="s">
-        <v>173</v>
-      </c>
       <c r="Z66" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA66" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG66" t="s">
         <v>115</v>
@@ -8615,12 +8212,6 @@
       <c r="U67" t="s">
         <v>443</v>
       </c>
-      <c r="V67" t="s">
-        <v>485</v>
-      </c>
-      <c r="W67" t="s">
-        <v>174</v>
-      </c>
       <c r="X67" t="s">
         <v>443</v>
       </c>
@@ -8628,22 +8219,22 @@
         <v>443</v>
       </c>
       <c r="Z67" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA67" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB67" t="s">
-        <v>551</v>
+        <v>524</v>
       </c>
       <c r="AC67" t="s">
-        <v>596</v>
+        <v>571</v>
       </c>
       <c r="AG67" t="s">
         <v>116</v>
       </c>
       <c r="AX67" t="s">
-        <v>835</v>
+        <v>794</v>
       </c>
     </row>
     <row r="68" spans="1:51" x14ac:dyDescent="0.2">
@@ -8707,12 +8298,6 @@
       <c r="U68" t="s">
         <v>443</v>
       </c>
-      <c r="V68" t="s">
-        <v>418</v>
-      </c>
-      <c r="W68" t="s">
-        <v>175</v>
-      </c>
       <c r="X68" t="s">
         <v>443</v>
       </c>
@@ -8720,55 +8305,55 @@
         <v>443</v>
       </c>
       <c r="Z68" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA68" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB68" t="s">
-        <v>552</v>
+        <v>525</v>
       </c>
       <c r="AC68" t="s">
-        <v>597</v>
+        <v>572</v>
       </c>
       <c r="AE68" t="s">
-        <v>647</v>
+        <v>622</v>
       </c>
       <c r="AG68" t="s">
         <v>117</v>
       </c>
       <c r="AJ68" t="s">
-        <v>695</v>
+        <v>651</v>
       </c>
       <c r="AK68" t="s">
-        <v>711</v>
+        <v>668</v>
       </c>
       <c r="AL68" t="s">
-        <v>725</v>
+        <v>682</v>
       </c>
       <c r="AM68" t="s">
+        <v>696</v>
+      </c>
+      <c r="AN68" t="s">
+        <v>712</v>
+      </c>
+      <c r="AO68" t="s">
+        <v>728</v>
+      </c>
+      <c r="AP68" t="s">
         <v>738</v>
       </c>
-      <c r="AN68" t="s">
-        <v>754</v>
-      </c>
-      <c r="AO68" t="s">
-        <v>770</v>
-      </c>
-      <c r="AP68" t="s">
-        <v>780</v>
-      </c>
       <c r="AQ68" t="s">
-        <v>790</v>
+        <v>749</v>
       </c>
       <c r="AR68" t="s">
-        <v>801</v>
+        <v>760</v>
       </c>
       <c r="AS68">
         <v>2013</v>
       </c>
       <c r="AX68" t="s">
-        <v>836</v>
+        <v>795</v>
       </c>
       <c r="AY68">
         <v>2016</v>
@@ -8820,47 +8405,41 @@
       <c r="U69" t="s">
         <v>443</v>
       </c>
-      <c r="V69" t="s">
-        <v>486</v>
-      </c>
-      <c r="W69" t="s">
-        <v>176</v>
-      </c>
       <c r="X69" t="s">
-        <v>500</v>
+        <v>470</v>
       </c>
       <c r="Y69" t="s">
-        <v>502</v>
+        <v>472</v>
       </c>
       <c r="Z69" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA69" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB69" t="s">
-        <v>553</v>
+        <v>526</v>
       </c>
       <c r="AC69" t="s">
-        <v>598</v>
+        <v>573</v>
       </c>
       <c r="AD69">
         <v>8606852046</v>
       </c>
       <c r="AE69" t="s">
-        <v>648</v>
+        <v>623</v>
       </c>
       <c r="AG69" t="s">
         <v>118</v>
       </c>
       <c r="AJ69" t="s">
-        <v>696</v>
+        <v>652</v>
       </c>
       <c r="AS69">
         <v>2016</v>
       </c>
       <c r="AX69" t="s">
-        <v>837</v>
+        <v>796</v>
       </c>
     </row>
     <row r="70" spans="1:51" x14ac:dyDescent="0.2">
@@ -8909,12 +8488,6 @@
       <c r="U70" t="s">
         <v>443</v>
       </c>
-      <c r="V70" t="s">
-        <v>487</v>
-      </c>
-      <c r="W70" t="s">
-        <v>177</v>
-      </c>
       <c r="X70" t="s">
         <v>443</v>
       </c>
@@ -8922,22 +8495,22 @@
         <v>443</v>
       </c>
       <c r="Z70" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AA70" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AB70" t="s">
-        <v>554</v>
+        <v>527</v>
       </c>
       <c r="AC70" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="AG70" t="s">
         <v>119</v>
       </c>
       <c r="AX70" t="s">
-        <v>825</v>
+        <v>784</v>
       </c>
     </row>
     <row r="71" spans="1:51" x14ac:dyDescent="0.2">
@@ -8963,7 +8536,7 @@
         <v>8085</v>
       </c>
       <c r="Z71" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="AG71" t="s">
         <v>120</v>
@@ -9012,26 +8585,20 @@
       <c r="O72">
         <v>8253</v>
       </c>
-      <c r="V72" t="s">
-        <v>488</v>
-      </c>
-      <c r="W72" t="s">
-        <v>178</v>
-      </c>
       <c r="AB72" t="s">
-        <v>488</v>
+        <v>528</v>
       </c>
       <c r="AC72" t="s">
         <v>178</v>
       </c>
       <c r="AD72" t="s">
-        <v>628</v>
+        <v>603</v>
       </c>
       <c r="AG72" t="s">
         <v>121</v>
       </c>
       <c r="AX72" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
     </row>
     <row r="73" spans="1:51" x14ac:dyDescent="0.2">
@@ -9057,13 +8624,13 @@
         <v>8415</v>
       </c>
       <c r="Z73" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="AG73" t="s">
         <v>122</v>
       </c>
       <c r="AY73" t="s">
-        <v>858</v>
+        <v>817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try to go back to a point where the Harvard-Marlboro issue was non-existent
Spoiler alert: It was always there. I just never noticed it.
</commit_message>
<xml_diff>
--- a/Updated Zone 1 Activity New.xlsx
+++ b/Updated Zone 1 Activity New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46B8C39-760D-0440-B444-CCA8CE896959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8725F6-F034-FD41-9C38-6A01FF408538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2858,14 +2858,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P46" workbookViewId="0">
-      <selection activeCell="V83" sqref="V83"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="22" max="22" width="43.33203125" customWidth="1"/>
-    <col min="23" max="23" width="53.33203125" customWidth="1"/>
+    <col min="17" max="17" width="47.6640625" customWidth="1"/>
+    <col min="22" max="22" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.2">

</xml_diff>